<commit_message>
Version estable 14-6 con mensajes programados correctamente
</commit_message>
<xml_diff>
--- a/registros/alertas.xlsx
+++ b/registros/alertas.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -91,7 +91,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -111,16 +111,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,17 +499,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="12.7109375" customWidth="1" style="1" min="1" max="1"/>
-    <col width="17.140625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="12.7109375" customWidth="1" min="3" max="6"/>
+    <col width="17.140625" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
+    <col width="12.7109375" customWidth="1" style="10" min="3" max="6"/>
     <col width="12.7109375" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -548,7 +550,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" s="10">
       <c r="A2" s="5" t="n">
         <v>45810</v>
       </c>
@@ -557,24 +559,24 @@
           <t>ADBE</t>
         </is>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="11" t="n">
         <v>401</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="11" t="n">
         <v>360.9</v>
       </c>
-      <c r="E2" s="10" t="n">
-        <v>396.7300109863281</v>
-      </c>
-      <c r="F2" s="10" t="n">
-        <v>416.7900085449219</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>0.0394</v>
-      </c>
-      <c r="H2" s="8" t="n"/>
-    </row>
-    <row r="3">
+      <c r="E2" s="11" t="n">
+        <v>383.75</v>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>391.2186889648438</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>-0.0244</v>
+      </c>
+      <c r="H2" s="12" t="n"/>
+    </row>
+    <row r="3" s="10">
       <c r="A3" s="5" t="n">
         <v>45810</v>
       </c>
@@ -583,24 +585,24 @@
           <t>LMT</t>
         </is>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="11" t="n">
         <v>475</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="11" t="n">
         <v>437</v>
       </c>
-      <c r="E3" s="10" t="n">
-        <v>471.75</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>478.5499877929688</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>0.0075</v>
-      </c>
-      <c r="H3" s="8" t="n"/>
-    </row>
-    <row r="4">
+      <c r="E3" s="11" t="n">
+        <v>443.4100036621094</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>484.010009765625</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H3" s="12" t="n"/>
+    </row>
+    <row r="4" s="10">
       <c r="A4" s="5" t="n">
         <v>45811</v>
       </c>
@@ -609,25 +611,25 @@
           <t>MSTR</t>
         </is>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="11" t="n">
         <v>382</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <f>+C4*0.88</f>
         <v/>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="11" t="n">
         <v>364.2999877929688</v>
       </c>
-      <c r="F4" s="10" t="n">
-        <v>379.3550109863281</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>-0.0069</v>
-      </c>
-      <c r="H4" s="8" t="n"/>
-    </row>
-    <row r="5">
+      <c r="F4" s="11" t="n">
+        <v>376.6600036621094</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>-0.014</v>
+      </c>
+      <c r="H4" s="12" t="n"/>
+    </row>
+    <row r="5" s="10">
       <c r="A5" s="5" t="n">
         <v>45811</v>
       </c>
@@ -636,24 +638,24 @@
           <t>GBAN.BA</t>
         </is>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="11" t="n">
         <v>2055</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="11" t="n">
         <v>1849.5</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E5" s="11" t="n">
         <v>1850</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="11" t="n">
         <v>2000</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="8" t="n">
         <v>-0.0268</v>
       </c>
-      <c r="H5" s="8" t="n"/>
-    </row>
-    <row r="6">
+      <c r="H5" s="12" t="n"/>
+    </row>
+    <row r="6" s="10">
       <c r="A6" s="5" t="n">
         <v>45811</v>
       </c>
@@ -662,24 +664,24 @@
           <t>METR.BA</t>
         </is>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="11" t="n">
         <v>2165</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="11" t="n">
         <v>1905.2</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="E6" s="11" t="n">
         <v>2020</v>
       </c>
-      <c r="F6" s="10" t="n">
-        <v>2125</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>-0.0185</v>
-      </c>
-      <c r="H6" s="8" t="n"/>
-    </row>
-    <row r="7">
+      <c r="F6" s="11" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>-0.037</v>
+      </c>
+      <c r="H6" s="12" t="n"/>
+    </row>
+    <row r="7" s="10">
       <c r="A7" s="5" t="n">
         <v>45813</v>
       </c>
@@ -688,275 +690,219 @@
           <t>COME.BA</t>
         </is>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="11" t="n">
         <v>149</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="11">
         <f>+C7*0.92</f>
         <v/>
       </c>
-      <c r="E7" s="10" t="n">
-        <v>143</v>
-      </c>
-      <c r="F7" s="10" t="n">
-        <v>145</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>-0.0268</v>
-      </c>
-      <c r="H7" s="8" t="n"/>
-    </row>
-    <row r="8">
+      <c r="E7" s="11" t="n">
+        <v>139.75</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>143.5</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>-0.0369</v>
+      </c>
+      <c r="H7" s="12" t="n"/>
+    </row>
+    <row r="8" s="10">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-10</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>FDX</t>
-        </is>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>216.73</v>
-      </c>
-      <c r="D8" s="10" t="n">
-        <v>185</v>
-      </c>
-      <c r="E8" s="10" t="n">
-        <v>219.1221923828125</v>
-      </c>
-      <c r="F8" s="10" t="n">
-        <v>220.0399932861328</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>0.0153</v>
-      </c>
-      <c r="H8" s="8" t="n"/>
-    </row>
-    <row r="9">
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>24.115</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>23.95999908447266</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>24.76499938964844</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="H8" s="12" t="n"/>
+    </row>
+    <row r="9" s="10">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-10</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>MU</t>
-        </is>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>106.29</v>
-      </c>
-      <c r="D9" s="10" t="n">
-        <v>99</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>108.0401000976562</v>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>110.629997253418</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>0.0408</v>
-      </c>
-      <c r="H9" s="8" t="n"/>
-    </row>
-    <row r="10">
+          <t>MIRG.BA</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>20625</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>19208</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>19500</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>20650</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="H9" s="12" t="n"/>
+    </row>
+    <row r="10" s="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>CGPA2.BA</t>
-        </is>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>2550</v>
-      </c>
-      <c r="D10" s="10" t="n">
-        <v>2210</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>2460</v>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>2505</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>-0.0176</v>
-      </c>
-      <c r="H10" s="8" t="n"/>
-    </row>
-    <row r="11">
+          <t>BYMA.BA</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>208.75</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>192</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>201</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>206.75</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="H10" s="12" t="n"/>
+    </row>
+    <row r="11" s="10">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
+          <t>MDT</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>88.06</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>75</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>87.76000213623047</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>88.45999908447266</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="H11" s="12" t="n"/>
+    </row>
+    <row r="12" s="10">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>2025-06-13</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>TLT</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>86.79000000000001</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>86.15000152587891</v>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>86.19000244140625</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <v>-0.0069</v>
+      </c>
+      <c r="H12" s="12" t="n"/>
+    </row>
+    <row r="13" s="10">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>2025-06-13</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
           <t>SAMI.BA</t>
         </is>
       </c>
-      <c r="C11" s="10" t="n">
-        <v>603</v>
-      </c>
-      <c r="D11" s="10" t="n">
-        <v>566</v>
-      </c>
-      <c r="E11" s="10" t="n">
-        <v>591</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>604</v>
-      </c>
-      <c r="G11" s="7" t="n">
-        <v>0.0017</v>
-      </c>
-      <c r="H11" s="8" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="n"/>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="10" t="n"/>
-      <c r="D12" s="10" t="n"/>
-      <c r="E12" s="10" t="n"/>
-      <c r="F12" s="10" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="8" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="n"/>
-      <c r="B13" s="6" t="n"/>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="10" t="n"/>
-      <c r="E13" s="10" t="n"/>
-      <c r="F13" s="10" t="n"/>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="8" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n"/>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="10" t="n"/>
-      <c r="D14" s="10" t="n"/>
-      <c r="E14" s="10" t="n"/>
-      <c r="F14" s="10" t="n"/>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="8" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="6" t="n"/>
-      <c r="C15" s="10" t="n"/>
-      <c r="D15" s="10" t="n"/>
-      <c r="E15" s="10" t="n"/>
-      <c r="F15" s="10" t="n"/>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="8" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="n"/>
-      <c r="B16" s="6" t="n"/>
-      <c r="C16" s="10" t="n"/>
-      <c r="D16" s="10" t="n"/>
-      <c r="E16" s="10" t="n"/>
-      <c r="F16" s="10" t="n"/>
-      <c r="G16" s="7" t="n"/>
-      <c r="H16" s="8" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="n"/>
-      <c r="B17" s="6" t="n"/>
-      <c r="C17" s="10" t="n"/>
-      <c r="D17" s="10" t="n"/>
-      <c r="E17" s="10" t="n"/>
-      <c r="F17" s="10" t="n"/>
-      <c r="G17" s="7" t="n"/>
-      <c r="H17" s="8" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="n"/>
-      <c r="B18" s="6" t="n"/>
-      <c r="C18" s="10" t="n"/>
-      <c r="D18" s="10" t="n"/>
-      <c r="E18" s="10" t="n"/>
-      <c r="F18" s="10" t="n"/>
-      <c r="G18" s="7" t="n"/>
-      <c r="H18" s="8" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="n"/>
-      <c r="B19" s="6" t="n"/>
-      <c r="C19" s="10" t="n"/>
-      <c r="D19" s="10" t="n"/>
-      <c r="E19" s="10" t="n"/>
-      <c r="F19" s="10" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="8" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="n"/>
-      <c r="B20" s="6" t="n"/>
-      <c r="C20" s="10" t="n"/>
-      <c r="D20" s="10" t="n"/>
-      <c r="E20" s="10" t="n"/>
-      <c r="F20" s="10" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="8" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="10" t="n"/>
-      <c r="E21" s="10" t="n"/>
-      <c r="F21" s="10" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="8" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="10" t="n"/>
-      <c r="E22" s="10" t="n"/>
-      <c r="F22" s="10" t="n"/>
-      <c r="G22" s="7" t="n"/>
-      <c r="H22" s="8" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="n"/>
-      <c r="B23" s="6" t="n"/>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="10" t="n"/>
-      <c r="E23" s="10" t="n"/>
-      <c r="F23" s="10" t="n"/>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="8" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="n"/>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="10" t="n"/>
-      <c r="E24" s="10" t="n"/>
-      <c r="F24" s="10" t="n"/>
-      <c r="G24" s="7" t="n"/>
-      <c r="H24" s="8" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="n"/>
-      <c r="B25" s="6" t="n"/>
-      <c r="C25" s="10" t="n"/>
-      <c r="D25" s="10" t="n"/>
-      <c r="E25" s="10" t="n"/>
-      <c r="F25" s="10" t="n"/>
-      <c r="G25" s="7" t="n"/>
-      <c r="H25" s="8" t="n"/>
+      <c r="C13" s="11" t="n">
+        <v>622</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>610</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>623</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="H13" s="12" t="n"/>
+    </row>
+    <row r="14" s="10">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>2025-06-13</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>HARG.BA</t>
+        </is>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>1630</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>1501</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>1550</v>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>-0.0184</v>
+      </c>
+      <c r="H14" s="12" t="n"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
@@ -965,9 +911,9 @@
     </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="num" val="-1.2"/>
-        <cfvo type="num" val="-0.1"/>
-        <cfvo type="num" val="0.8"/>
+        <cfvo type="num" val="-0.2"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.2"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>